<commit_message>
fixing regex auto intervention
</commit_message>
<xml_diff>
--- a/experimentresources/interventionsauto/emptytemplate.xlsx
+++ b/experimentresources/interventionsauto/emptytemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chattoolTG\experimentresources\interventionsauto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02AEDD6-1B4E-40C5-AD91-E606D8C0D7CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EAE94E-1082-42C8-B0F6-8A3990FF92E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5856" yWindow="6732" windowWidth="26496" windowHeight="19128" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14904" yWindow="7512" windowWidth="26568" windowHeight="20844" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="explanation" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4573" uniqueCount="4556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4573" uniqueCount="4557">
   <si>
     <t>P1ID</t>
   </si>
@@ -13693,10 +13693,13 @@
     <t>This spreadsheet allows you to specify rules for blocking and / or modifying participants' turns.  There are three sheets: block, modify and delay. Edit the text to specify the rules. The chattool first checks to see if the turn is to be blocked. If not, it processes the rules from top-to-bottom of the  "modify" sheet and then processed from top to bottom of the "delay" sheet.  Note that these rules work with the Telegram and the Turn By Turn Interface (not yet with the WYSIWYG Interface)</t>
   </si>
   <si>
-    <t>\d</t>
-  </si>
-  <si>
-    <t>DIGIT</t>
+    <t>\b[a]\b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>AAAAA</t>
   </si>
 </sst>
 </file>
@@ -22733,11 +22736,11 @@
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
       <c r="J8" t="s">
-        <v>4554</v>
+        <v>4555</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="3" t="s">
-        <v>4555</v>
+        <v>4556</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="8"/>

</xml_diff>